<commit_message>
update task gen file
</commit_message>
<xml_diff>
--- a/Task1-feature_generation.xlsx
+++ b/Task1-feature_generation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somani4\Documents\GitHub\ECE498_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67745589-6687-4C32-B3FF-42674C4BC6A5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76868A83-AB23-41D3-B1D5-4CE2F5544FDC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="4" xr2:uid="{6979EBDE-FDCA-4B42-918E-2C70D40B6D11}"/>
   </bookViews>
@@ -1095,14 +1095,13 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="14"/>
       <color rgb="FF002060"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1118,6 +1117,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1180,7 +1191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1207,10 +1218,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1228,13 +1235,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2571,8 +2591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364DD11A-90DE-054D-9738-15F07178DAD1}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2582,31 +2602,31 @@
     <col min="3" max="3" width="70.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="28" customFormat="1" ht="16" thickBot="1">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:6" s="30" customFormat="1" ht="18.5" thickBot="1">
+      <c r="A1" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" s="32" customFormat="1">
+      <c r="A2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2618,7 +2638,7 @@
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2630,7 +2650,7 @@
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2641,7 +2661,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2652,7 +2672,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2663,7 +2683,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2674,7 +2694,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2685,7 +2705,7 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="26" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2696,26 +2716,26 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="18" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="18" customFormat="1">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:6" s="36" customFormat="1">
+      <c r="A12" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="35" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="26" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2726,7 +2746,7 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="18" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -2737,7 +2757,7 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2747,32 +2767,32 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:6" s="32" customFormat="1">
+      <c r="A16" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="37" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="17" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="18" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2783,7 +2803,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -2794,7 +2814,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="18" t="s">
         <v>67</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2804,24 +2824,24 @@
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:3" s="32" customFormat="1">
+      <c r="A22" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="38" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="18" t="s">
         <v>70</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2832,40 +2852,40 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="26" t="s">
         <v>80</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="20" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="19" t="s">
         <v>81</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="21" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="19" t="s">
         <v>82</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="22" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="26" t="s">
         <v>85</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2876,7 +2896,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2886,38 +2906,38 @@
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="18" customFormat="1">
-      <c r="A30" s="21" t="s">
+    <row r="30" spans="1:3" s="16" customFormat="1">
+      <c r="A30" s="19" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="18" customFormat="1">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:3" s="16" customFormat="1">
+      <c r="A31" s="18" t="s">
         <v>101</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="23" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="18" customFormat="1">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:3" s="16" customFormat="1">
+      <c r="A32" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="23" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="18" t="s">
         <v>103</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2928,7 +2948,7 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="19" t="s">
         <v>107</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -2939,7 +2959,7 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="26" t="s">
         <v>108</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2950,7 +2970,7 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="19" t="s">
         <v>116</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -2961,7 +2981,7 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="26" t="s">
         <v>117</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -2972,7 +2992,7 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="26" t="s">
         <v>118</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -3037,10 +3057,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.5">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3">

</xml_diff>